<commit_message>
-done actualizations in the gantt_final.xlsx file -added gant diagramm to document LogicielStructureSkyguide.docx
</commit_message>
<xml_diff>
--- a/_documents/phase2/gantt_final.xlsx
+++ b/_documents/phase2/gantt_final.xlsx
@@ -11,6 +11,10 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$3:$AF$42</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Feuil1!$A:$A,Feuil1!$4:$5</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -261,9 +265,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -272,6 +273,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -579,7 +583,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AB39" sqref="AB39"/>
+      <selection pane="bottomRight" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,15 +729,15 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="20" t="s">
         <v>14</v>
       </c>
       <c r="U6" s="4"/>
       <c r="Z6" s="4"/>
-      <c r="AC6" s="12" t="s">
+      <c r="AC6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AD6" s="12" t="s">
+      <c r="AD6" s="20" t="s">
         <v>37</v>
       </c>
       <c r="AE6" s="4"/>
@@ -743,17 +747,17 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="12"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="12"/>
+      <c r="N7" s="20"/>
       <c r="U7" s="4"/>
       <c r="Z7" s="4"/>
-      <c r="AC7" s="12"/>
-      <c r="AD7" s="12"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
     </row>
@@ -761,17 +765,17 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="13"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="12"/>
+      <c r="N8" s="20"/>
       <c r="U8" s="4"/>
       <c r="Z8" s="4"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="12"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
     </row>
@@ -779,18 +783,18 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="12"/>
+      <c r="N9" s="20"/>
       <c r="U9" s="4"/>
       <c r="Z9" s="4"/>
-      <c r="AC9" s="12"/>
-      <c r="AD9" s="12"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
     </row>
@@ -800,15 +804,15 @@
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="13"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="12"/>
+      <c r="N10" s="20"/>
       <c r="U10" s="4"/>
       <c r="Z10" s="4"/>
-      <c r="AC10" s="12"/>
-      <c r="AD10" s="12"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
     </row>
@@ -818,16 +822,16 @@
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="I11" s="14"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="6"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="12"/>
+      <c r="N11" s="20"/>
       <c r="U11" s="4"/>
       <c r="Z11" s="4"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="12"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20"/>
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
     </row>
@@ -840,13 +844,13 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="12"/>
+      <c r="N12" s="20"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="U12" s="4"/>
       <c r="Z12" s="4"/>
-      <c r="AC12" s="12"/>
-      <c r="AD12" s="12"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
     </row>
@@ -859,7 +863,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="12"/>
+      <c r="N13" s="20"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -868,8 +872,8 @@
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
       <c r="Z13" s="4"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="20"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
     </row>
@@ -882,15 +886,15 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="12"/>
+      <c r="N14" s="20"/>
       <c r="U14" s="4"/>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="4"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="12"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
     </row>
@@ -905,11 +909,11 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="12"/>
+      <c r="N15" s="20"/>
       <c r="U15" s="4"/>
       <c r="Z15" s="4"/>
-      <c r="AC15" s="12"/>
-      <c r="AD15" s="12"/>
+      <c r="AC15" s="20"/>
+      <c r="AD15" s="20"/>
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
     </row>
@@ -917,20 +921,20 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="12"/>
+      <c r="N16" s="20"/>
       <c r="U16" s="4"/>
       <c r="Z16" s="4"/>
-      <c r="AC16" s="12"/>
-      <c r="AD16" s="12"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="20"/>
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
     </row>
@@ -940,19 +944,19 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="12"/>
+      <c r="N17" s="20"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="U17" s="4"/>
       <c r="Z17" s="4"/>
-      <c r="AC17" s="12"/>
-      <c r="AD17" s="12"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20"/>
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
     </row>
@@ -966,11 +970,11 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="12"/>
+      <c r="N18" s="20"/>
       <c r="U18" s="4"/>
       <c r="Z18" s="4"/>
-      <c r="AC18" s="12"/>
-      <c r="AD18" s="12"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20"/>
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
     </row>
@@ -983,15 +987,15 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="12"/>
+      <c r="N19" s="20"/>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
       <c r="U19" s="4"/>
       <c r="V19" s="8"/>
       <c r="Z19" s="4"/>
-      <c r="AC19" s="12"/>
-      <c r="AD19" s="12"/>
+      <c r="AC19" s="20"/>
+      <c r="AD19" s="20"/>
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
     </row>
@@ -1004,13 +1008,13 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="12"/>
+      <c r="N20" s="20"/>
       <c r="W20" s="8"/>
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
       <c r="Z20" s="4"/>
-      <c r="AC20" s="12"/>
-      <c r="AD20" s="12"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="20"/>
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
     </row>
@@ -1023,13 +1027,13 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="12"/>
+      <c r="N21" s="20"/>
       <c r="U21" s="4"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="8"/>
       <c r="AB21" s="8"/>
-      <c r="AC21" s="12"/>
-      <c r="AD21" s="12"/>
+      <c r="AC21" s="20"/>
+      <c r="AD21" s="20"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
     </row>
@@ -1043,11 +1047,11 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="12"/>
+      <c r="N22" s="20"/>
       <c r="U22" s="4"/>
       <c r="Z22" s="4"/>
-      <c r="AC22" s="12"/>
-      <c r="AD22" s="12"/>
+      <c r="AC22" s="20"/>
+      <c r="AD22" s="20"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
     </row>
@@ -1055,20 +1059,20 @@
       <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="12"/>
+      <c r="N23" s="20"/>
       <c r="U23" s="4"/>
       <c r="Z23" s="4"/>
-      <c r="AC23" s="12"/>
-      <c r="AD23" s="12"/>
+      <c r="AC23" s="20"/>
+      <c r="AD23" s="20"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
     </row>
@@ -1078,16 +1082,16 @@
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="12"/>
+      <c r="N24" s="20"/>
       <c r="U24" s="4"/>
       <c r="Z24" s="4"/>
-      <c r="AC24" s="12"/>
-      <c r="AD24" s="12"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="20"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
     </row>
@@ -1101,11 +1105,11 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="12"/>
+      <c r="N25" s="20"/>
       <c r="U25" s="4"/>
       <c r="Z25" s="4"/>
-      <c r="AC25" s="12"/>
-      <c r="AD25" s="12"/>
+      <c r="AC25" s="20"/>
+      <c r="AD25" s="20"/>
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
     </row>
@@ -1118,7 +1122,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="12"/>
+      <c r="N26" s="20"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
@@ -1129,8 +1133,8 @@
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="Z26" s="4"/>
-      <c r="AC26" s="12"/>
-      <c r="AD26" s="12"/>
+      <c r="AC26" s="20"/>
+      <c r="AD26" s="20"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
     </row>
@@ -1143,15 +1147,15 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="12"/>
+      <c r="N27" s="20"/>
       <c r="U27" s="4"/>
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="4"/>
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
-      <c r="AC27" s="12"/>
-      <c r="AD27" s="12"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="20"/>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
     </row>
@@ -1164,11 +1168,11 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="12"/>
+      <c r="N28" s="20"/>
       <c r="U28" s="4"/>
       <c r="Z28" s="4"/>
-      <c r="AC28" s="12"/>
-      <c r="AD28" s="12"/>
+      <c r="AC28" s="20"/>
+      <c r="AD28" s="20"/>
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
     </row>
@@ -1176,18 +1180,18 @@
       <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="12"/>
+      <c r="N29" s="20"/>
       <c r="U29" s="4"/>
       <c r="Z29" s="4"/>
-      <c r="AC29" s="12"/>
-      <c r="AD29" s="12"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20"/>
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
     </row>
@@ -1195,17 +1199,17 @@
       <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="18"/>
+      <c r="D30" s="17"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="12"/>
+      <c r="N30" s="20"/>
       <c r="U30" s="4"/>
       <c r="Z30" s="4"/>
-      <c r="AC30" s="12"/>
-      <c r="AD30" s="12"/>
+      <c r="AC30" s="20"/>
+      <c r="AD30" s="20"/>
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
     </row>
@@ -1213,18 +1217,18 @@
       <c r="A31" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="18"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="18"/>
+      <c r="H31" s="17"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="12"/>
+      <c r="N31" s="20"/>
       <c r="U31" s="4"/>
       <c r="Z31" s="4"/>
-      <c r="AC31" s="12"/>
-      <c r="AD31" s="12"/>
+      <c r="AC31" s="20"/>
+      <c r="AD31" s="20"/>
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
     </row>
@@ -1234,15 +1238,15 @@
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="I32" s="18"/>
+      <c r="I32" s="17"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="12"/>
+      <c r="N32" s="20"/>
       <c r="U32" s="4"/>
       <c r="Z32" s="4"/>
-      <c r="AC32" s="12"/>
-      <c r="AD32" s="12"/>
+      <c r="AC32" s="20"/>
+      <c r="AD32" s="20"/>
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
     </row>
@@ -1256,11 +1260,11 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
-      <c r="N33" s="12"/>
+      <c r="N33" s="20"/>
       <c r="U33" s="4"/>
       <c r="Z33" s="4"/>
-      <c r="AC33" s="12"/>
-      <c r="AD33" s="12"/>
+      <c r="AC33" s="20"/>
+      <c r="AD33" s="20"/>
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
     </row>
@@ -1273,7 +1277,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="12"/>
+      <c r="N34" s="20"/>
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
@@ -1284,8 +1288,8 @@
       <c r="V34" s="10"/>
       <c r="W34" s="10"/>
       <c r="Z34" s="4"/>
-      <c r="AC34" s="12"/>
-      <c r="AD34" s="12"/>
+      <c r="AC34" s="20"/>
+      <c r="AD34" s="20"/>
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
     </row>
@@ -1298,15 +1302,15 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
-      <c r="N35" s="12"/>
+      <c r="N35" s="20"/>
       <c r="U35" s="4"/>
       <c r="X35" s="10"/>
       <c r="Y35" s="10"/>
       <c r="Z35" s="4"/>
       <c r="AA35" s="10"/>
       <c r="AB35" s="10"/>
-      <c r="AC35" s="12"/>
-      <c r="AD35" s="12"/>
+      <c r="AC35" s="20"/>
+      <c r="AD35" s="20"/>
       <c r="AE35" s="4"/>
       <c r="AF35" s="4"/>
     </row>
@@ -1319,11 +1323,11 @@
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
-      <c r="N36" s="12"/>
+      <c r="N36" s="20"/>
       <c r="U36" s="4"/>
       <c r="Z36" s="4"/>
-      <c r="AC36" s="12"/>
-      <c r="AD36" s="12"/>
+      <c r="AC36" s="20"/>
+      <c r="AD36" s="20"/>
       <c r="AE36" s="4"/>
       <c r="AF36" s="4"/>
     </row>
@@ -1331,20 +1335,20 @@
       <c r="A37" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="18"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
-      <c r="N37" s="12"/>
+      <c r="N37" s="20"/>
       <c r="U37" s="4"/>
       <c r="Z37" s="4"/>
-      <c r="AC37" s="12"/>
-      <c r="AD37" s="12"/>
+      <c r="AC37" s="20"/>
+      <c r="AD37" s="20"/>
       <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
     </row>
@@ -1354,16 +1358,16 @@
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="20"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="19"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
-      <c r="N38" s="12"/>
+      <c r="N38" s="20"/>
       <c r="U38" s="4"/>
       <c r="Z38" s="4"/>
-      <c r="AC38" s="12"/>
-      <c r="AD38" s="12"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="20"/>
       <c r="AE38" s="4"/>
       <c r="AF38" s="4"/>
     </row>
@@ -1376,7 +1380,7 @@
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
-      <c r="N39" s="12"/>
+      <c r="N39" s="20"/>
       <c r="O39" s="11"/>
       <c r="P39" s="11"/>
       <c r="Q39" s="11"/>
@@ -1391,8 +1395,8 @@
       <c r="Z39" s="4"/>
       <c r="AA39" s="11"/>
       <c r="AB39" s="11"/>
-      <c r="AC39" s="12"/>
-      <c r="AD39" s="12"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
       <c r="AE39" s="4"/>
       <c r="AF39" s="4"/>
     </row>
@@ -1406,11 +1410,11 @@
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
-      <c r="N40" s="12"/>
+      <c r="N40" s="20"/>
       <c r="U40" s="4"/>
       <c r="Z40" s="4"/>
-      <c r="AC40" s="12"/>
-      <c r="AD40" s="12"/>
+      <c r="AC40" s="20"/>
+      <c r="AD40" s="20"/>
       <c r="AE40" s="4"/>
       <c r="AF40" s="4"/>
     </row>
@@ -1420,11 +1424,11 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="12"/>
+      <c r="N41" s="20"/>
       <c r="U41" s="4"/>
       <c r="Z41" s="4"/>
-      <c r="AC41" s="12"/>
-      <c r="AD41" s="12"/>
+      <c r="AC41" s="20"/>
+      <c r="AD41" s="20"/>
       <c r="AE41" s="4"/>
       <c r="AF41" s="4"/>
     </row>
@@ -1434,11 +1438,11 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="12"/>
+      <c r="N42" s="20"/>
       <c r="U42" s="4"/>
       <c r="Z42" s="4"/>
-      <c r="AC42" s="12"/>
-      <c r="AD42" s="12"/>
+      <c r="AC42" s="20"/>
+      <c r="AD42" s="20"/>
       <c r="AE42" s="4"/>
       <c r="AF42" s="4"/>
     </row>
@@ -1448,8 +1452,8 @@
     <mergeCell ref="AC6:AC42"/>
     <mergeCell ref="AD6:AD42"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="60" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>